<commit_message>
Added exercises on Skewness and Variance
</commit_message>
<xml_diff>
--- a/resources/Part_3_Statistics/S15_L84/2.8.Skewness-exercise.xlsx
+++ b/resources/Part_3_Statistics/S15_L84/2.8.Skewness-exercise.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Skewness" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Skewness!$L$10:$L$39</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Skewness!$B$10:$B$39</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Skewness</t>
   </si>
@@ -53,6 +57,45 @@
   </si>
   <si>
     <t>Identify the skewness of dataset 2. You may use the formula from the lesson, the skewness formula in excel (=SKEW) or you can plot it on a graph</t>
+  </si>
+  <si>
+    <t>Formula:</t>
+  </si>
+  <si>
+    <t>n=</t>
+  </si>
+  <si>
+    <t>x media=</t>
+  </si>
+  <si>
+    <t>POTENCIA</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>N:</t>
+  </si>
+  <si>
+    <t>X Media</t>
+  </si>
+  <si>
+    <t>Xi - Xmedia</t>
+  </si>
+  <si>
+    <t>al cubo</t>
+  </si>
+  <si>
+    <t>X 1/n</t>
+  </si>
+  <si>
+    <t>Al cuadrado</t>
+  </si>
+  <si>
+    <t>X 1/(n-1)</t>
+  </si>
+  <si>
+    <t>Raiz cúbica</t>
   </si>
 </sst>
 </file>
@@ -123,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -132,6 +175,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,6 +193,1189 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{F6606196-86F7-4021-ABBD-233D4B79DCE4}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r" underflow="auto" overflow="auto">
+              <cx:binCount val="8"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{F3F28D71-C8C5-4F6C-90C4-6F24AAFEE651}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="8"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Gráfico 2"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,25 +1641,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O39"/>
+  <dimension ref="B1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="1"/>
-    <col min="5" max="5" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -438,7 +1674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -446,7 +1682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -454,10 +1690,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
     </row>
-    <row r="9" spans="2:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="O8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
@@ -470,253 +1717,966 @@
       <c r="N9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <f>SKEW(L10:L39)</f>
+        <v>-0.37064131089909302</v>
+      </c>
+      <c r="T9" s="1">
+        <f>Q41/U41</f>
+        <v>-120325.91253685816</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>212</v>
       </c>
+      <c r="C10" s="1">
+        <f>POWER(B10-$E$12, 3)</f>
+        <v>-3946808.9267037055</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1">
+        <f>POWER(B10-$E$12,2)</f>
+        <v>24974.534444444453</v>
+      </c>
+      <c r="H10" s="1">
+        <f>1/E11*C40</f>
+        <v>10470284.096740736</v>
+      </c>
       <c r="L10" s="1">
         <v>586</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+      <c r="M10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="1">
+        <f>COUNT(L10:L39)</f>
+        <v>30</v>
+      </c>
+      <c r="O10" s="1">
+        <f>L10-$N$11</f>
+        <v>-17.733333333333348</v>
+      </c>
+      <c r="P10" s="1">
+        <f>O10^3</f>
+        <v>-5576.6210370370518</v>
+      </c>
+      <c r="R10" s="1">
+        <f>O10^2</f>
+        <v>314.47111111111167</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>869</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:C39" si="0">POWER(B11-$E$12, 3)</f>
+        <v>124226600.56329627</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <f>COUNT(B10:B39)</f>
+        <v>30</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" ref="F11:F39" si="1">POWER(B11-$E$12,2)</f>
+        <v>248967.73444444442</v>
+      </c>
+      <c r="H11" s="1">
+        <f>((1/(E11-1))*F40)^(1/3)</f>
+        <v>41.149148505929006</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <f>H10/H11</f>
+        <v>254447.16298885545</v>
+      </c>
       <c r="L11" s="1">
         <v>760</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="2">
+        <f>SUM(L10:L39)/N10</f>
+        <v>603.73333333333335</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O39" si="2">L11-$N$11</f>
+        <v>156.26666666666665</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" ref="P11:P39" si="3">O11^3</f>
+        <v>3815918.0989629617</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" ref="R11:R39" si="4">O11^2</f>
+        <v>24419.271111111106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>220</v>
       </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>-3377250.5000370392</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SUM(B10:B39)/E11</f>
+        <v>370.03333333333336</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>22510.00111111112</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SKEW(B10:B39)</f>
+        <v>0.63098801196505716</v>
+      </c>
       <c r="L12" s="1">
         <v>495</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O12" s="1">
+        <f t="shared" si="2"/>
+        <v>-108.73333333333335</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="3"/>
+        <v>-1285547.4343703708</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="4"/>
+        <v>11822.937777777781</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>654</v>
       </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>22898239.346629623</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>80637.06777777776</v>
+      </c>
       <c r="L13" s="1">
         <v>678</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O13" s="1">
+        <f t="shared" si="2"/>
+        <v>74.266666666666652</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="3"/>
+        <v>409620.6056296294</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="4"/>
+        <v>5515.5377777777758</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>511</v>
       </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>2801233.3699629614</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>19871.601111111104</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="1">
+        <f>POWER(H11,1/3)</f>
+        <v>3.4523934523856221</v>
+      </c>
       <c r="L14" s="1">
         <v>559</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O14" s="1">
+        <f t="shared" si="2"/>
+        <v>-44.733333333333348</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>-89514.581037037133</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="4"/>
+        <v>2001.0711111111125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>624</v>
       </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>16380613.246629626</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>64499.067777777767</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1">
+        <f>H11^(1/3)</f>
+        <v>3.4523934523856221</v>
+      </c>
       <c r="L15" s="1">
         <v>415</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="O15" s="1">
+        <f t="shared" si="2"/>
+        <v>-188.73333333333335</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="3"/>
+        <v>-6722732.5010370389</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="4"/>
+        <v>35620.27111111112</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>420</v>
       </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>124750.16662962943</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>2496.667777777775</v>
+      </c>
       <c r="L16" s="1">
         <v>370</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O16" s="1">
+        <f t="shared" si="2"/>
+        <v>-233.73333333333335</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="3"/>
+        <v>-12769149.10103704</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="4"/>
+        <v>54631.27111111112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>121</v>
       </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>-15444449.930037042</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>62017.601111111122</v>
+      </c>
       <c r="L17" s="1">
         <v>659</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O17" s="1">
+        <f t="shared" si="2"/>
+        <v>55.266666666666652</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="3"/>
+        <v>168806.75229629615</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="4"/>
+        <v>3054.4044444444426</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>428</v>
       </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>194775.79329629603</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>3360.1344444444412</v>
+      </c>
       <c r="L18" s="1">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O18" s="1">
+        <f t="shared" si="2"/>
+        <v>-484.73333333333335</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="3"/>
+        <v>-113896048.44770372</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="4"/>
+        <v>234966.40444444446</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>865</v>
       </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>121262874.14996295</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>244992.00111111108</v>
+      </c>
       <c r="L19" s="1">
         <v>288</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O19" s="1">
+        <f t="shared" si="2"/>
+        <v>-315.73333333333335</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="3"/>
+        <v>-31474678.594370376</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="4"/>
+        <v>99687.53777777779</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>799</v>
       </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>78935186.329962939</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>184012.40111111107</v>
+      </c>
       <c r="L20" s="1">
         <v>241</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O20" s="1">
+        <f t="shared" si="2"/>
+        <v>-362.73333333333335</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="3"/>
+        <v>-47726809.221037038</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="4"/>
+        <v>131575.47111111111</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>405</v>
       </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>42752.616629629534</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>1222.6677777777759</v>
+      </c>
       <c r="L21" s="1">
         <v>787</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O21" s="1">
+        <f t="shared" si="2"/>
+        <v>183.26666666666665</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="3"/>
+        <v>6155317.2589629618</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="4"/>
+        <v>33586.671111111107</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>230</v>
       </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>-2745960.4667037055</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>19609.334444444452</v>
+      </c>
       <c r="L22" s="1">
         <v>522</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O22" s="1">
+        <f t="shared" si="2"/>
+        <v>-81.733333333333348</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="3"/>
+        <v>-546006.27437037067</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="4"/>
+        <v>6680.3377777777805</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>670</v>
       </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>26991000.999962956</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>89980.001111111094</v>
+      </c>
       <c r="L23" s="1">
         <v>207</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O23" s="1">
+        <f t="shared" si="2"/>
+        <v>-396.73333333333335</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="3"/>
+        <v>-62444770.474370375</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" si="4"/>
+        <v>157397.33777777778</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>870</v>
       </c>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>124975001.6666296</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>249966.66777777774</v>
+      </c>
       <c r="L24" s="1">
         <v>160</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O24" s="1">
+        <f t="shared" si="2"/>
+        <v>-443.73333333333335</v>
+      </c>
+      <c r="P24" s="1">
+        <f t="shared" si="3"/>
+        <v>-87370769.901037052</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="4"/>
+        <v>196899.27111111113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>366</v>
       </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>-65.613370370371655</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>16.26777777777799</v>
+      </c>
       <c r="L25" s="1">
         <v>526</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O25" s="1">
+        <f t="shared" si="2"/>
+        <v>-77.733333333333348</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" si="3"/>
+        <v>-469701.42103703733</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" si="4"/>
+        <v>6042.4711111111137</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>99</v>
       </c>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>-19909856.003370374</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>73459.067777777789</v>
+      </c>
       <c r="L26" s="1">
         <v>656</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O26" s="1">
+        <f t="shared" si="2"/>
+        <v>52.266666666666652</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" si="3"/>
+        <v>142782.31229629615</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" si="4"/>
+        <v>2731.8044444444427</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>55</v>
       </c>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>-31265798.550037045</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>99246.001111111123</v>
+      </c>
       <c r="L27" s="1">
         <v>848</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O27" s="1">
+        <f t="shared" si="2"/>
+        <v>244.26666666666665</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" si="3"/>
+        <v>14574464.872296294</v>
+      </c>
+      <c r="R27" s="1">
+        <f t="shared" si="4"/>
+        <v>59666.20444444444</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>489</v>
       </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>1683743.2966296284</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>14153.067777777771</v>
+      </c>
       <c r="L28" s="1">
         <v>720</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O28" s="1">
+        <f t="shared" si="2"/>
+        <v>116.26666666666665</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" si="3"/>
+        <v>1571685.565629629</v>
+      </c>
+      <c r="R28" s="1">
+        <f t="shared" si="4"/>
+        <v>13517.937777777774</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>312</v>
       </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>-195448.59337037063</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>3367.8677777777807</v>
+      </c>
       <c r="L29" s="1">
         <v>676</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O29" s="1">
+        <f t="shared" si="2"/>
+        <v>72.266666666666652</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" si="3"/>
+        <v>377410.57896296273</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" si="4"/>
+        <v>5222.4711111111092</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>493</v>
       </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>1859354.5099629618</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="1"/>
+        <v>15120.801111111105</v>
+      </c>
       <c r="L30" s="1">
         <v>581</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O30" s="1">
+        <f t="shared" si="2"/>
+        <v>-22.733333333333348</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" si="3"/>
+        <v>-11748.687703703728</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="4"/>
+        <v>516.80444444444515</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>163</v>
       </c>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>-8874028.5900370404</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>42862.801111111119</v>
+      </c>
       <c r="L31" s="1">
         <v>929</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O31" s="1">
+        <f t="shared" si="2"/>
+        <v>325.26666666666665</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" si="3"/>
+        <v>34412694.352296293</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="4"/>
+        <v>105798.40444444443</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>221</v>
       </c>
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>-3310169.5967037058</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>22210.934444444454</v>
+      </c>
       <c r="L32" s="1">
         <v>653</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O32" s="1">
+        <f t="shared" si="2"/>
+        <v>49.266666666666652</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" si="3"/>
+        <v>119580.27229629617</v>
+      </c>
+      <c r="R32" s="1">
+        <f t="shared" si="4"/>
+        <v>2427.2044444444427</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
         <v>84</v>
       </c>
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>-23401836.553370375</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>81815.067777777789</v>
+      </c>
       <c r="L33" s="1">
         <v>661</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O33" s="1">
+        <f t="shared" si="2"/>
+        <v>57.266666666666652</v>
+      </c>
+      <c r="P33" s="1">
+        <f t="shared" si="3"/>
+        <v>187804.3789629628</v>
+      </c>
+      <c r="R33" s="1">
+        <f t="shared" si="4"/>
+        <v>3279.4711111111092</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
         <v>144</v>
       </c>
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>-11548284.353370374</v>
+      </c>
+      <c r="F34" s="1">
+        <f t="shared" si="1"/>
+        <v>51091.067777777789</v>
+      </c>
       <c r="L34" s="1">
         <v>770</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O34" s="1">
+        <f t="shared" si="2"/>
+        <v>166.26666666666665</v>
+      </c>
+      <c r="P34" s="1">
+        <f t="shared" si="3"/>
+        <v>4596376.2322962945</v>
+      </c>
+      <c r="R34" s="1">
+        <f t="shared" si="4"/>
+        <v>27644.604444444438</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B35" s="1">
         <v>48</v>
       </c>
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>-33396617.473370381</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="1"/>
+        <v>103705.4677777778</v>
+      </c>
       <c r="L35" s="1">
         <v>800</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O35" s="1">
+        <f t="shared" si="2"/>
+        <v>196.26666666666665</v>
+      </c>
+      <c r="P35" s="1">
+        <f t="shared" si="3"/>
+        <v>7560310.6322962949</v>
+      </c>
+      <c r="R35" s="1">
+        <f t="shared" si="4"/>
+        <v>38520.604444444441</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B36" s="1">
         <v>375</v>
       </c>
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>122.51662962962766</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="1"/>
+        <v>24.667777777777513</v>
+      </c>
       <c r="L36" s="1">
         <v>529</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O36" s="1">
+        <f t="shared" si="2"/>
+        <v>-74.733333333333348</v>
+      </c>
+      <c r="P36" s="1">
+        <f t="shared" si="3"/>
+        <v>-417390.98103703727</v>
+      </c>
+      <c r="R36" s="1">
+        <f t="shared" si="4"/>
+        <v>5585.0711111111132</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B37" s="1">
         <v>86</v>
       </c>
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>-22914370.546703711</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="1"/>
+        <v>80674.934444444458</v>
+      </c>
       <c r="L37" s="1">
         <v>975</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O37" s="1">
+        <f t="shared" si="2"/>
+        <v>371.26666666666665</v>
+      </c>
+      <c r="P37" s="1">
+        <f t="shared" si="3"/>
+        <v>51175002.965629622</v>
+      </c>
+      <c r="R37" s="1">
+        <f t="shared" si="4"/>
+        <v>137838.93777777776</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B38" s="1">
         <v>168</v>
       </c>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>-8246489.0733703738</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="1"/>
+        <v>40817.467777777791</v>
+      </c>
       <c r="L38" s="1">
         <v>995</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="O38" s="1">
+        <f t="shared" si="2"/>
+        <v>391.26666666666665</v>
+      </c>
+      <c r="P38" s="1">
+        <f t="shared" si="3"/>
+        <v>59898859.232296295</v>
+      </c>
+      <c r="R38" s="1">
+        <f t="shared" si="4"/>
+        <v>153089.60444444444</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B39" s="1">
         <v>100</v>
       </c>
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>-19690290.900037043</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="1"/>
+        <v>72918.001111111123</v>
+      </c>
       <c r="L39" s="1">
         <v>947</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="2"/>
+        <v>343.26666666666665</v>
+      </c>
+      <c r="P39" s="1">
+        <f t="shared" si="3"/>
+        <v>40447799.392296292</v>
+      </c>
+      <c r="R39" s="1">
+        <f t="shared" si="4"/>
+        <v>117832.00444444444</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C40" s="1">
+        <f>SUM(C10:C39)</f>
+        <v>314108522.9022221</v>
+      </c>
+      <c r="F40" s="1">
+        <f>SUM(F10:F39)</f>
+        <v>2020600.9666666668</v>
+      </c>
+      <c r="P40" s="1">
+        <f>SUM(P10:P39)</f>
+        <v>-139616010.73777786</v>
+      </c>
+      <c r="R40" s="1">
+        <f>SUM(R10:R39)</f>
+        <v>1677885.8666666667</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q41" s="1">
+        <f>(1/N10)*P40</f>
+        <v>-4653867.0245925952</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="1">
+        <f>(1/(N10-1)*R40)</f>
+        <v>57858.133333333331</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U41" s="1">
+        <f>S41^(1/3)</f>
+        <v>38.677180388447297</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>